<commit_message>
Lastest on 6th Nov
</commit_message>
<xml_diff>
--- a/InputData.xlsx
+++ b/InputData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7EC0C4-66EB-4F1F-8219-CF5FDA589FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB9C6D4-7BED-409C-839E-EF15856866FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>https://www.amazon.com/s?k=gaming+headsets&amp;pd_rd_r=97e61485-3ef8-4c14-9d2a-2868c19b31b1&amp;pd_rd_w=UsXP9&amp;pd_rd_wg=Y2QyM&amp;pf_rd_p=12129333-2117-4490-9c17-6d31baf0582a&amp;pf_rd_r=4ATEYRKJ9QPB33SMND9E&amp;ref=pd_gw_unk</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/s?k=gaming+keyboard&amp;pd_rd_r=27df3aff-f7ce-49f0-8c9e-fd59d881145f&amp;pd_rd_w=Wr12F&amp;pd_rd_wg=Y9Ors&amp;pf_rd_p=12129333-2117-4490-9c17-6d31baf0582a&amp;pf_rd_r=YQ1M6XJGJ4B5453YSDMX&amp;ref=pd_gw_unk</t>
   </si>
 </sst>
 </file>
@@ -340,10 +343,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -353,6 +356,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>